<commit_message>
Finalize Task: Mrbeast-analysis: Modify the content of groundtruth and format to better fit the task description. Optimize the evaluation process. Update prompt to be more clear and comprehensive.
</commit_message>
<xml_diff>
--- a/tasks/finalpool/mrbeast-analysis/initial_workspace/result.xlsx
+++ b/tasks/finalpool/mrbeast-analysis/initial_workspace/result.xlsx
@@ -1,52 +1,114 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quentin/Desktop/RESEARCH/MCP/finalpool/mcpbench_dev/tasks/finalpool/mrbeast-analysis/initial_workspace/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCA9769-9CCB-974B-B29F-409412DE541A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-740" yWindow="-20980" windowWidth="10980" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Detail_Lists" sheetId="1" r:id="rId1"/>
     <sheet name="Statics" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>video_id</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>published_at(ISO 8601 format)</t>
+  </si>
+  <si>
+    <t>duration_seconds</t>
+  </si>
+  <si>
+    <t>weekday</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Most_common_publish_weekday</t>
+  </si>
+  <si>
+    <t>Saturday_publish_proportion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thursday_publish_proportion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Friday_publish_proportion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wednesday_publish_proportion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tuesday_publish_proportion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monday_publish_proportion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sunday_publish_proportion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Statistic_Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average_duration_excluding_shorts(HH:MM:SS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average_publish_interval(days)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>duration_formatted(HH:MM:SS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>category</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="6">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -71,13 +133,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -402,105 +472,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>video_id</v>
-      </c>
-      <c r="B1" t="str">
-        <v>title</v>
-      </c>
-      <c r="C1" t="str">
-        <v>published_at(ISO 8601 format)</v>
-      </c>
-      <c r="D1" t="str">
-        <v>duration_seconds</v>
-      </c>
-      <c r="E1" t="str">
-        <v>duration_formatted(xx:xx:xx)</v>
-      </c>
-      <c r="F1" t="str">
-        <v>published_date</v>
-      </c>
-      <c r="G1" t="str">
-        <v>weekday</v>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G1"/>
+    <ignoredError sqref="D1:E1 G1 A1:B1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Statistic_Item</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Value</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Most_common_publish_weekday</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Average_duration_excluding_shorts(HH:MM:SS)</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Average_publish_interval(days)</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Saturday_publish_frequency</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Thursday_publish_frequency</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Friday_publish_frequency</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Wednesday_publish_frequency</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Tuesday_publish_frequency</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>Monday_publish_frequency</v>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B10"/>
+    <ignoredError sqref="A2:B2 B11 B6 B8 B9 B10 B1 B4 B3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: course-assistant & mrbeast-analysis
</commit_message>
<xml_diff>
--- a/tasks/finalpool/mrbeast-analysis/initial_workspace/result.xlsx
+++ b/tasks/finalpool/mrbeast-analysis/initial_workspace/result.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quentin/Desktop/RESEARCH/MCP/finalpool/mcpbench_dev/tasks/finalpool/mrbeast-analysis/initial_workspace/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lockon\Desktop\toolathlon\mrbeast-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCA9769-9CCB-974B-B29F-409412DE541A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C919B1-867B-4514-A9BA-6ADBDA9358E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-740" yWindow="-20980" windowWidth="10980" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-65685" yWindow="1845" windowWidth="22785" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detail_Lists" sheetId="1" r:id="rId1"/>
-    <sheet name="Statics" sheetId="2" r:id="rId2"/>
+    <sheet name="Statistics" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -96,7 +96,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -475,13 +475,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -517,13 +517,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -531,52 +531,52 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>12</v>
       </c>

</xml_diff>